<commit_message>
Final Commit of the Day 2/2
</commit_message>
<xml_diff>
--- a/src/main/java/TestSuite/MDOT/Scenarios/MDOT/TS_PM_COA_SEC_AgencyObjectProfile_Regression_001.xlsx
+++ b/src/main/java/TestSuite/MDOT/Scenarios/MDOT/TS_PM_COA_SEC_AgencyObjectProfile_Regression_001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdighe\Documents\MDOT\rstars\src\main\java\TestSuite\MDOT\Scenarios\MDOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490FBF77-B1AB-4359-A8B2-150CA18413B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F37105C-4F00-4A57-B10A-5149BE8F3835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -842,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="3">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>